<commit_message>
Added deserialization, read, dual-mode filtering
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Projects\nevermore\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" activeTab="4"/>
+    <workbookView activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Metas" sheetId="2" r:id="rId2"/>
-    <sheet name="Metas1" sheetId="3" r:id="rId3"/>
-    <sheet name="Metas2" sheetId="4" r:id="rId4"/>
-    <sheet name="TestModels" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Metas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Metas1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Metas2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TestModels" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>_id</t>
   </si>
@@ -42,26 +37,37 @@
   <si>
     <t>Brian</t>
   </si>
+  <si>
+    <t>Rob</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt formatCode="m/d/yy\ h:mm;@" numFmtId="164"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <i val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,26 +83,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -384,32 +385,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" width="10.5546875"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,86 +431,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>43046.5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="n">
         <v>43046.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>43047</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="n">
         <v>43047</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="n">
         <v>43048</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>43048</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="n">
         <v>43049</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>43049</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>43050</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="n">
         <v>43050</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="n">
         <v>43051</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>43051</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,19 +537,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,56 +576,84 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C5" pane="bottomLeft" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="4.109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="2" style="5" width="12.5546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="6.21875"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="4.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row customFormat="1" r="1" s="2" spans="1:5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>43047.198366104851</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43047.198366104851</v>
+      <c r="B2" s="5" t="n">
+        <v>43047.19836610485</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>43047.19836805556</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>43058.05815972222</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>43058.2549537037</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>